<commit_message>
- temp version for save code
</commit_message>
<xml_diff>
--- a/shared/config.xlsx
+++ b/shared/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zyh/work/my-code/happy-fish/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF04BCC-C2C7-9B4A-8743-9B3E6661102F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC61C67-EFDB-5E49-AA6A-88141F018E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="28520" windowHeight="19260" activeTab="4" xr2:uid="{05761CE9-AD8C-CC45-98B7-3A5E92D6F1D4}"/>
+    <workbookView xWindow="2120" yWindow="460" windowWidth="28520" windowHeight="19260" activeTab="5" xr2:uid="{05761CE9-AD8C-CC45-98B7-3A5E92D6F1D4}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="room" sheetId="4" r:id="rId3"/>
     <sheet name="activity" sheetId="5" r:id="rId4"/>
     <sheet name="weapon" sheetId="3" r:id="rId5"/>
+    <sheet name="tween" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -308,6 +309,154 @@
   </si>
   <si>
     <t>[{"x":100,"y":2,"seconds":4},{"x":400,"y":-2,"seconds":10},{"x":1800,"y":0,"seconds":10}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缓动函数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>smooth</t>
+  </si>
+  <si>
+    <t>fade</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>quadIn</t>
+  </si>
+  <si>
+    <t>quadOut</t>
+  </si>
+  <si>
+    <t>quadInOut</t>
+  </si>
+  <si>
+    <t>quadOutIn</t>
+  </si>
+  <si>
+    <t>cubicIn</t>
+  </si>
+  <si>
+    <t>cubicOut</t>
+  </si>
+  <si>
+    <t>cubicInOut</t>
+  </si>
+  <si>
+    <t>cubicOutIn</t>
+  </si>
+  <si>
+    <t>quartIn</t>
+  </si>
+  <si>
+    <t>quartOut</t>
+  </si>
+  <si>
+    <t>quartInOut</t>
+  </si>
+  <si>
+    <t>quartOutIn</t>
+  </si>
+  <si>
+    <t>quintIn</t>
+  </si>
+  <si>
+    <t>quintOut</t>
+  </si>
+  <si>
+    <t>quintInOut</t>
+  </si>
+  <si>
+    <t>quintOutIn</t>
+  </si>
+  <si>
+    <t>sineIn</t>
+  </si>
+  <si>
+    <t>sineOut</t>
+  </si>
+  <si>
+    <t>sineInOut</t>
+  </si>
+  <si>
+    <t>sineOutIn</t>
+  </si>
+  <si>
+    <t>expoIn</t>
+  </si>
+  <si>
+    <t>expoOut</t>
+  </si>
+  <si>
+    <t>expoInOut</t>
+  </si>
+  <si>
+    <t>expoOutIn</t>
+  </si>
+  <si>
+    <t>circIn</t>
+  </si>
+  <si>
+    <t>circOut</t>
+  </si>
+  <si>
+    <t>circInOut</t>
+  </si>
+  <si>
+    <t>circOutIn</t>
+  </si>
+  <si>
+    <t>elasticIn</t>
+  </si>
+  <si>
+    <t>elasticOut</t>
+  </si>
+  <si>
+    <t>elasticInOut</t>
+  </si>
+  <si>
+    <t>elasticOutIn</t>
+  </si>
+  <si>
+    <t>backIn</t>
+  </si>
+  <si>
+    <t>backOut</t>
+  </si>
+  <si>
+    <t>backInOut</t>
+  </si>
+  <si>
+    <t>backOutIn</t>
+  </si>
+  <si>
+    <t>bounceIn</t>
+  </si>
+  <si>
+    <t>bounceOut</t>
+  </si>
+  <si>
+    <t>bounceInOut</t>
+  </si>
+  <si>
+    <t>bounceOutIn</t>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1267,7 +1416,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1279,156 +1428,440 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085074B5-4ACD-F148-9F0F-9C014A079E83}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="54" customHeight="1">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="54" customHeight="1">
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>36</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>40</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>40</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>50</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>60</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>70</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C310139-0454-824F-9A8A-74E0C7100104}">
+  <dimension ref="A1:A47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- animation - stand up / down - rename
</commit_message>
<xml_diff>
--- a/shared/config.xlsx
+++ b/shared/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zyh/work/my-code/happy-fish/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC61C67-EFDB-5E49-AA6A-88141F018E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B91CD5-9FB9-B446-851C-9F7078EF7B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="28520" windowHeight="19260" activeTab="5" xr2:uid="{05761CE9-AD8C-CC45-98B7-3A5E92D6F1D4}"/>
+    <workbookView xWindow="4120" yWindow="1820" windowWidth="28520" windowHeight="19260" activeTab="5" xr2:uid="{05761CE9-AD8C-CC45-98B7-3A5E92D6F1D4}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fish_denglong</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fish_yellow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -320,143 +316,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>linear</t>
-  </si>
-  <si>
-    <t>smooth</t>
-  </si>
-  <si>
-    <t>fade</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
-    <t>quadIn</t>
-  </si>
-  <si>
-    <t>quadOut</t>
-  </si>
-  <si>
-    <t>quadInOut</t>
-  </si>
-  <si>
-    <t>quadOutIn</t>
-  </si>
-  <si>
-    <t>cubicIn</t>
-  </si>
-  <si>
-    <t>cubicOut</t>
-  </si>
-  <si>
-    <t>cubicInOut</t>
-  </si>
-  <si>
-    <t>cubicOutIn</t>
-  </si>
-  <si>
-    <t>quartIn</t>
-  </si>
-  <si>
-    <t>quartOut</t>
-  </si>
-  <si>
-    <t>quartInOut</t>
-  </si>
-  <si>
-    <t>quartOutIn</t>
-  </si>
-  <si>
-    <t>quintIn</t>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fish_denglongyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>circOut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>quintOut</t>
-  </si>
-  <si>
-    <t>quintInOut</t>
-  </si>
-  <si>
-    <t>quintOutIn</t>
-  </si>
-  <si>
-    <t>sineIn</t>
-  </si>
-  <si>
-    <t>sineOut</t>
-  </si>
-  <si>
-    <t>sineInOut</t>
-  </si>
-  <si>
-    <t>sineOutIn</t>
-  </si>
-  <si>
-    <t>expoIn</t>
-  </si>
-  <si>
-    <t>expoOut</t>
-  </si>
-  <si>
-    <t>expoInOut</t>
-  </si>
-  <si>
-    <t>expoOutIn</t>
-  </si>
-  <si>
-    <t>circIn</t>
-  </si>
-  <si>
-    <t>circOut</t>
-  </si>
-  <si>
-    <t>circInOut</t>
-  </si>
-  <si>
-    <t>circOutIn</t>
-  </si>
-  <si>
-    <t>elasticIn</t>
-  </si>
-  <si>
-    <t>elasticOut</t>
-  </si>
-  <si>
-    <t>elasticInOut</t>
-  </si>
-  <si>
-    <t>elasticOutIn</t>
-  </si>
-  <si>
-    <t>backIn</t>
-  </si>
-  <si>
-    <t>backOut</t>
-  </si>
-  <si>
-    <t>backInOut</t>
-  </si>
-  <si>
-    <t>backOutIn</t>
-  </si>
-  <si>
-    <t>bounceIn</t>
-  </si>
-  <si>
-    <t>bounceOut</t>
-  </si>
-  <si>
-    <t>bounceInOut</t>
-  </si>
-  <si>
-    <t>bounceOutIn</t>
-  </si>
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -846,7 +722,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -857,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -866,13 +742,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -906,13 +782,13 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -940,7 +816,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -960,7 +836,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -980,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -1000,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -1020,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -1040,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>30</v>
@@ -1060,7 +936,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>40</v>
@@ -1080,7 +956,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>40</v>
@@ -1100,7 +976,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>80</v>
@@ -1120,7 +996,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>50</v>
@@ -1156,13 +1032,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1173,18 +1049,18 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="65" customHeight="1">
@@ -1192,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="88" customHeight="1">
@@ -1203,10 +1079,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="72" customHeight="1">
@@ -1214,10 +1090,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="70" customHeight="1">
@@ -1225,10 +1101,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="57" customHeight="1">
@@ -1236,10 +1112,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="52" customHeight="1">
@@ -1247,10 +1123,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="65" customHeight="1">
@@ -1258,10 +1134,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="43" customHeight="1"/>
@@ -1287,22 +1163,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1319,30 +1195,30 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" customHeight="1">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1350,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>100000</v>
@@ -1362,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1370,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3">
         <v>2000000</v>
@@ -1382,7 +1258,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1390,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>60000000</v>
@@ -1402,7 +1278,7 @@
         <v>600</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1442,19 +1318,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1476,19 +1352,19 @@
     </row>
     <row r="3" spans="1:5" ht="54" customHeight="1">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1499,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1516,7 +1392,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -1533,7 +1409,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -1550,7 +1426,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -1567,7 +1443,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1584,7 +1460,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>60</v>
@@ -1601,7 +1477,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>70</v>
@@ -1618,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C310139-0454-824F-9A8A-74E0C7100104}">
-  <dimension ref="A1:A47"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1631,7 +1507,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1641,227 +1517,17 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>